<commit_message>
Finalized and ready to use first version
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1133,7 +1133,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1154,7 +1154,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1238,7 +1238,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1301,7 +1301,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">

</xml_diff>